<commit_message>
small update on some dataset
</commit_message>
<xml_diff>
--- a/spreadsheet/web_scrape_hammer.xlsx
+++ b/spreadsheet/web_scrape_hammer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamlam/Desktop/FYP/ObjectPropertiesInformationExtraction/spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594D1996-A771-044D-B498-1007200DAE0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A225D10-6573-374A-97AF-655762089703}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="22100" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2250" uniqueCount="1152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2250" uniqueCount="1151">
   <si>
     <t>Input</t>
   </si>
@@ -9391,9 +9391,6 @@
   </si>
   <si>
     <t>11.6</t>
-  </si>
-  <si>
-    <t>steel</t>
   </si>
   <si>
     <t>5.67kg</t>
@@ -10359,8 +10356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="F178" sqref="F178"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14132,19 +14129,19 @@
         <v>322</v>
       </c>
       <c r="D118" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="F118" s="1" t="s">
         <v>956</v>
       </c>
-      <c r="E118" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="F118" s="1" t="s">
+      <c r="G118" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H118" s="1" t="s">
         <v>957</v>
-      </c>
-      <c r="G118" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H118" s="1" t="s">
-        <v>958</v>
       </c>
       <c r="I118" s="1" t="s">
         <v>844</v>
@@ -14176,10 +14173,10 @@
         <v>656</v>
       </c>
       <c r="H119" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="I119" s="1" t="s">
         <v>959</v>
-      </c>
-      <c r="I119" s="1" t="s">
-        <v>960</v>
       </c>
       <c r="J119" s="1" t="s">
         <v>822</v>
@@ -14196,22 +14193,22 @@
         <v>328</v>
       </c>
       <c r="D120" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="F120" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="E120" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="F120" s="1" t="s">
+      <c r="G120" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H120" s="1" t="s">
         <v>962</v>
       </c>
-      <c r="G120" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H120" s="1" t="s">
+      <c r="I120" s="1" t="s">
         <v>963</v>
-      </c>
-      <c r="I120" s="1" t="s">
-        <v>964</v>
       </c>
       <c r="J120" s="1" t="s">
         <v>688</v>
@@ -14240,7 +14237,7 @@
         <v>656</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I121" s="1" t="s">
         <v>844</v>
@@ -14266,13 +14263,13 @@
         <v>656</v>
       </c>
       <c r="F122" s="1" t="s">
+        <v>965</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H122" s="1" t="s">
         <v>966</v>
-      </c>
-      <c r="G122" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H122" s="1" t="s">
-        <v>967</v>
       </c>
       <c r="I122" s="1" t="s">
         <v>921</v>
@@ -14298,7 +14295,7 @@
         <v>656</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>656</v>
@@ -14307,7 +14304,7 @@
         <v>716</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="J123" s="1" t="s">
         <v>870</v>
@@ -14330,7 +14327,7 @@
         <v>656</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>809</v>
@@ -14342,7 +14339,7 @@
         <v>896</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="125" spans="1:10" ht="256" x14ac:dyDescent="0.2">
@@ -14362,7 +14359,7 @@
         <v>656</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>656</v>
@@ -14371,10 +14368,10 @@
         <v>945</v>
       </c>
       <c r="I125" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="J125" s="1" t="s">
         <v>973</v>
-      </c>
-      <c r="J125" s="1" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="126" spans="1:10" ht="335" x14ac:dyDescent="0.2">
@@ -14394,19 +14391,19 @@
         <v>779</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="G126" s="1" t="s">
         <v>793</v>
       </c>
       <c r="H126" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="I126" s="1" t="s">
         <v>976</v>
       </c>
-      <c r="I126" s="1" t="s">
+      <c r="J126" s="1" t="s">
         <v>977</v>
-      </c>
-      <c r="J126" s="1" t="s">
-        <v>978</v>
       </c>
     </row>
     <row r="127" spans="1:10" ht="304" x14ac:dyDescent="0.2">
@@ -14426,10 +14423,10 @@
         <v>741</v>
       </c>
       <c r="F127" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="G127" s="1" t="s">
         <v>979</v>
-      </c>
-      <c r="G127" s="1" t="s">
-        <v>980</v>
       </c>
       <c r="H127" s="1" t="s">
         <v>727</v>
@@ -14458,7 +14455,7 @@
         <v>656</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>677</v>
@@ -14467,7 +14464,7 @@
         <v>756</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="J128" s="1" t="s">
         <v>811</v>
@@ -14490,16 +14487,16 @@
         <v>656</v>
       </c>
       <c r="F129" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="G129" s="1" t="s">
         <v>983</v>
       </c>
-      <c r="G129" s="1" t="s">
+      <c r="H129" s="1" t="s">
         <v>984</v>
       </c>
-      <c r="H129" s="1" t="s">
+      <c r="I129" s="1" t="s">
         <v>985</v>
-      </c>
-      <c r="I129" s="1" t="s">
-        <v>986</v>
       </c>
       <c r="J129" s="1" t="s">
         <v>673</v>
@@ -14554,16 +14551,16 @@
         <v>656</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="G131" s="1" t="s">
         <v>755</v>
       </c>
       <c r="H131" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="I131" s="1" t="s">
         <v>988</v>
-      </c>
-      <c r="I131" s="1" t="s">
-        <v>989</v>
       </c>
       <c r="J131" s="1" t="s">
         <v>727</v>
@@ -14586,16 +14583,16 @@
         <v>656</v>
       </c>
       <c r="F132" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="G132" s="1" t="s">
         <v>990</v>
       </c>
-      <c r="G132" s="1" t="s">
+      <c r="H132" s="1" t="s">
         <v>991</v>
       </c>
-      <c r="H132" s="1" t="s">
+      <c r="I132" s="1" t="s">
         <v>992</v>
-      </c>
-      <c r="I132" s="1" t="s">
-        <v>993</v>
       </c>
       <c r="J132" s="1" t="s">
         <v>896</v>
@@ -14618,7 +14615,7 @@
         <v>656</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="G133" s="1" t="s">
         <v>809</v>
@@ -14630,7 +14627,7 @@
         <v>771</v>
       </c>
       <c r="J133" s="1" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="134" spans="1:10" ht="192" x14ac:dyDescent="0.2">
@@ -14656,13 +14653,13 @@
         <v>656</v>
       </c>
       <c r="H134" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="I134" s="1" t="s">
         <v>996</v>
       </c>
-      <c r="I134" s="1" t="s">
+      <c r="J134" s="1" t="s">
         <v>997</v>
-      </c>
-      <c r="J134" s="1" t="s">
-        <v>998</v>
       </c>
     </row>
     <row r="135" spans="1:10" ht="112" x14ac:dyDescent="0.2">
@@ -14682,10 +14679,10 @@
         <v>656</v>
       </c>
       <c r="F135" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="G135" s="1" t="s">
         <v>999</v>
-      </c>
-      <c r="G135" s="1" t="s">
-        <v>1000</v>
       </c>
       <c r="H135" s="1" t="s">
         <v>851</v>
@@ -14720,10 +14717,10 @@
         <v>663</v>
       </c>
       <c r="H136" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I136" s="1" t="s">
         <v>1001</v>
-      </c>
-      <c r="I136" s="1" t="s">
-        <v>1002</v>
       </c>
       <c r="J136" s="1" t="s">
         <v>708</v>
@@ -14746,7 +14743,7 @@
         <v>656</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="G137" s="1" t="s">
         <v>677</v>
@@ -14755,7 +14752,7 @@
         <v>802</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="J137" s="1" t="s">
         <v>855</v>
@@ -14778,7 +14775,7 @@
         <v>656</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="G138" s="1" t="s">
         <v>656</v>
@@ -14810,7 +14807,7 @@
         <v>656</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="G139" s="1" t="s">
         <v>656</v>
@@ -14842,13 +14839,13 @@
         <v>656</v>
       </c>
       <c r="F140" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="G140" s="1" t="s">
         <v>1006</v>
       </c>
-      <c r="G140" s="1" t="s">
+      <c r="H140" s="1" t="s">
         <v>1007</v>
-      </c>
-      <c r="H140" s="1" t="s">
-        <v>1008</v>
       </c>
       <c r="I140" s="1" t="s">
         <v>691</v>
@@ -14874,7 +14871,7 @@
         <v>656</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="G141" s="1" t="s">
         <v>656</v>
@@ -14883,10 +14880,10 @@
         <v>675</v>
       </c>
       <c r="I141" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="J141" s="1" t="s">
         <v>1010</v>
-      </c>
-      <c r="J141" s="1" t="s">
-        <v>1011</v>
       </c>
     </row>
     <row r="142" spans="1:10" ht="335" x14ac:dyDescent="0.2">
@@ -14906,19 +14903,19 @@
         <v>656</v>
       </c>
       <c r="F142" s="1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="G142" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H142" s="1" t="s">
         <v>1012</v>
       </c>
-      <c r="G142" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H142" s="1" t="s">
+      <c r="I142" s="1" t="s">
         <v>1013</v>
       </c>
-      <c r="I142" s="1" t="s">
+      <c r="J142" s="1" t="s">
         <v>1014</v>
-      </c>
-      <c r="J142" s="1" t="s">
-        <v>1015</v>
       </c>
     </row>
     <row r="143" spans="1:10" ht="304" x14ac:dyDescent="0.2">
@@ -14932,25 +14929,25 @@
         <v>397</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>779</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="G143" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H143" s="1" t="s">
         <v>1016</v>
       </c>
-      <c r="H143" s="1" t="s">
+      <c r="I143" s="1" t="s">
         <v>1017</v>
       </c>
-      <c r="I143" s="1" t="s">
+      <c r="J143" s="1" t="s">
         <v>1018</v>
-      </c>
-      <c r="J143" s="1" t="s">
-        <v>1019</v>
       </c>
     </row>
     <row r="144" spans="1:10" ht="288" x14ac:dyDescent="0.2">
@@ -14976,7 +14973,7 @@
         <v>755</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="I144" s="1" t="s">
         <v>757</v>
@@ -15014,7 +15011,7 @@
         <v>748</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="146" spans="1:10" ht="320" x14ac:dyDescent="0.2">
@@ -15034,7 +15031,7 @@
         <v>656</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="G146" s="1" t="s">
         <v>656</v>
@@ -15095,16 +15092,16 @@
         <v>661</v>
       </c>
       <c r="E148" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F148" s="1" t="s">
         <v>1023</v>
-      </c>
-      <c r="F148" s="1" t="s">
-        <v>1024</v>
       </c>
       <c r="G148" s="1" t="s">
         <v>759</v>
       </c>
       <c r="H148" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I148" s="1" t="s">
         <v>704</v>
@@ -15139,10 +15136,10 @@
         <v>925</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="J149" s="1" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="150" spans="1:10" ht="272" x14ac:dyDescent="0.2">
@@ -15162,19 +15159,19 @@
         <v>656</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G150" s="1" t="s">
         <v>735</v>
       </c>
       <c r="H150" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="I150" s="1" t="s">
         <v>1027</v>
       </c>
-      <c r="I150" s="1" t="s">
+      <c r="J150" s="1" t="s">
         <v>1028</v>
-      </c>
-      <c r="J150" s="1" t="s">
-        <v>1029</v>
       </c>
     </row>
     <row r="151" spans="1:10" ht="304" x14ac:dyDescent="0.2">
@@ -15206,7 +15203,7 @@
         <v>709</v>
       </c>
       <c r="J151" s="1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="152" spans="1:10" ht="395" x14ac:dyDescent="0.2">
@@ -15258,16 +15255,16 @@
         <v>656</v>
       </c>
       <c r="F153" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="G153" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H153" s="1" t="s">
         <v>1031</v>
       </c>
-      <c r="G153" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H153" s="1" t="s">
+      <c r="I153" s="1" t="s">
         <v>1032</v>
-      </c>
-      <c r="I153" s="1" t="s">
-        <v>1033</v>
       </c>
       <c r="J153" s="1" t="s">
         <v>714</v>
@@ -15290,7 +15287,7 @@
         <v>656</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="G154" s="1" t="s">
         <v>876</v>
@@ -15328,13 +15325,13 @@
         <v>656</v>
       </c>
       <c r="H155" s="1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="I155" s="1" t="s">
         <v>1035</v>
       </c>
-      <c r="I155" s="1" t="s">
+      <c r="J155" s="1" t="s">
         <v>1036</v>
-      </c>
-      <c r="J155" s="1" t="s">
-        <v>1037</v>
       </c>
     </row>
     <row r="156" spans="1:10" ht="335" x14ac:dyDescent="0.2">
@@ -15360,13 +15357,13 @@
         <v>876</v>
       </c>
       <c r="H156" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="I156" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="J156" s="1" t="s">
         <v>1038</v>
-      </c>
-      <c r="I156" s="1" t="s">
-        <v>971</v>
-      </c>
-      <c r="J156" s="1" t="s">
-        <v>1039</v>
       </c>
     </row>
     <row r="157" spans="1:10" ht="320" x14ac:dyDescent="0.2">
@@ -15392,7 +15389,7 @@
         <v>735</v>
       </c>
       <c r="H157" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="I157" s="1" t="s">
         <v>748</v>
@@ -15418,13 +15415,13 @@
         <v>656</v>
       </c>
       <c r="F158" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="G158" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H158" s="1" t="s">
         <v>1041</v>
-      </c>
-      <c r="G158" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H158" s="1" t="s">
-        <v>1042</v>
       </c>
       <c r="I158" s="1" t="s">
         <v>904</v>
@@ -15456,10 +15453,10 @@
         <v>735</v>
       </c>
       <c r="H159" s="1" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="I159" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="J159" s="1" t="s">
         <v>748</v>
@@ -15482,7 +15479,7 @@
         <v>656</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="G160" s="1" t="s">
         <v>759</v>
@@ -15491,7 +15488,7 @@
         <v>665</v>
       </c>
       <c r="I160" s="1" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="J160" s="1" t="s">
         <v>877</v>
@@ -15514,19 +15511,19 @@
         <v>656</v>
       </c>
       <c r="F161" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="G161" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H161" s="1" t="s">
         <v>1045</v>
-      </c>
-      <c r="G161" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H161" s="1" t="s">
-        <v>1046</v>
       </c>
       <c r="I161" s="1" t="s">
         <v>955</v>
       </c>
       <c r="J161" s="1" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="162" spans="1:10" ht="288" x14ac:dyDescent="0.2">
@@ -15540,13 +15537,13 @@
         <v>454</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>656</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="G162" s="1" t="s">
         <v>656</v>
@@ -15555,10 +15552,10 @@
         <v>669</v>
       </c>
       <c r="I162" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="J162" s="1" t="s">
         <v>1048</v>
-      </c>
-      <c r="J162" s="1" t="s">
-        <v>1049</v>
       </c>
     </row>
     <row r="163" spans="1:10" ht="380" x14ac:dyDescent="0.2">
@@ -15578,7 +15575,7 @@
         <v>656</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="G163" s="1" t="s">
         <v>656</v>
@@ -15587,10 +15584,10 @@
         <v>776</v>
       </c>
       <c r="I163" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="J163" s="1" t="s">
         <v>1051</v>
-      </c>
-      <c r="J163" s="1" t="s">
-        <v>1052</v>
       </c>
     </row>
     <row r="164" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
@@ -15610,13 +15607,13 @@
         <v>741</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="G164" s="1" t="s">
         <v>656</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="I164" s="1" t="s">
         <v>664</v>
@@ -15642,7 +15639,7 @@
         <v>656</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="G165" s="1" t="s">
         <v>755</v>
@@ -15654,7 +15651,7 @@
         <v>771</v>
       </c>
       <c r="J165" s="1" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="166" spans="1:10" ht="272" x14ac:dyDescent="0.2">
@@ -15674,19 +15671,19 @@
         <v>656</v>
       </c>
       <c r="F166" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="G166" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H166" s="1" t="s">
         <v>1055</v>
-      </c>
-      <c r="G166" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H166" s="1" t="s">
-        <v>1056</v>
       </c>
       <c r="I166" s="1" t="s">
         <v>777</v>
       </c>
       <c r="J166" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="167" spans="1:10" ht="335" x14ac:dyDescent="0.2">
@@ -15700,22 +15697,22 @@
         <v>469</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E167" s="1" t="s">
         <v>656</v>
       </c>
       <c r="F167" s="1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H167" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="I167" s="1" t="s">
         <v>1058</v>
-      </c>
-      <c r="G167" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H167" s="1" t="s">
-        <v>1017</v>
-      </c>
-      <c r="I167" s="1" t="s">
-        <v>1059</v>
       </c>
       <c r="J167" s="1" t="s">
         <v>675</v>
@@ -15738,7 +15735,7 @@
         <v>741</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="G168" s="1" t="s">
         <v>677</v>
@@ -15750,7 +15747,7 @@
         <v>748</v>
       </c>
       <c r="J168" s="1" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="169" spans="1:10" ht="272" x14ac:dyDescent="0.2">
@@ -15776,10 +15773,10 @@
         <v>809</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I169" s="1" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="J169" s="1" t="s">
         <v>748</v>
@@ -15802,7 +15799,7 @@
         <v>656</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="G170" s="1" t="s">
         <v>656</v>
@@ -15837,7 +15834,7 @@
         <v>656</v>
       </c>
       <c r="G171" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="H171" s="1" t="s">
         <v>656</v>
@@ -15866,19 +15863,19 @@
         <v>656</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="G172" s="1" t="s">
         <v>663</v>
       </c>
       <c r="H172" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I172" s="1" t="s">
         <v>1065</v>
       </c>
-      <c r="I172" s="1" t="s">
-        <v>1066</v>
-      </c>
       <c r="J172" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="173" spans="1:10" ht="208" x14ac:dyDescent="0.2">
@@ -15898,13 +15895,13 @@
         <v>656</v>
       </c>
       <c r="F173" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="G173" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H173" s="1" t="s">
         <v>1067</v>
-      </c>
-      <c r="G173" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H173" s="1" t="s">
-        <v>1068</v>
       </c>
       <c r="I173" s="1" t="s">
         <v>678</v>
@@ -15930,16 +15927,16 @@
         <v>741</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="G174" s="1" t="s">
         <v>735</v>
       </c>
       <c r="H174" s="1" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="I174" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="J174" s="1" t="s">
         <v>748</v>
@@ -15962,16 +15959,16 @@
         <v>656</v>
       </c>
       <c r="F175" s="1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="G175" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H175" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="I175" s="1" t="s">
         <v>1070</v>
-      </c>
-      <c r="G175" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H175" s="1" t="s">
-        <v>1052</v>
-      </c>
-      <c r="I175" s="1" t="s">
-        <v>1071</v>
       </c>
       <c r="J175" s="1" t="s">
         <v>877</v>
@@ -15994,7 +15991,7 @@
         <v>656</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="G176" s="1" t="s">
         <v>656</v>
@@ -16006,7 +16003,7 @@
         <v>945</v>
       </c>
       <c r="J176" s="1" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="177" spans="1:10" ht="240" x14ac:dyDescent="0.2">
@@ -16026,13 +16023,13 @@
         <v>656</v>
       </c>
       <c r="F177" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H177" s="1" t="s">
         <v>1074</v>
-      </c>
-      <c r="G177" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H177" s="1" t="s">
-        <v>1075</v>
       </c>
       <c r="I177" s="1" t="s">
         <v>678</v>
@@ -16064,10 +16061,10 @@
         <v>656</v>
       </c>
       <c r="H178" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="I178" s="1" t="s">
         <v>1076</v>
-      </c>
-      <c r="I178" s="1" t="s">
-        <v>1077</v>
       </c>
       <c r="J178" s="1" t="s">
         <v>805</v>
@@ -16090,7 +16087,7 @@
         <v>656</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="G179" s="1" t="s">
         <v>656</v>
@@ -16102,7 +16099,7 @@
         <v>716</v>
       </c>
       <c r="J179" s="1" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="180" spans="1:10" ht="365" x14ac:dyDescent="0.2">
@@ -16122,13 +16119,13 @@
         <v>656</v>
       </c>
       <c r="F180" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G180" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H180" s="1" t="s">
         <v>1080</v>
-      </c>
-      <c r="G180" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H180" s="1" t="s">
-        <v>1081</v>
       </c>
       <c r="I180" s="1" t="s">
         <v>822</v>
@@ -16154,7 +16151,7 @@
         <v>656</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="G181" s="1" t="s">
         <v>656</v>
@@ -16186,7 +16183,7 @@
         <v>656</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="G182" s="1" t="s">
         <v>656</v>
@@ -16195,10 +16192,10 @@
         <v>842</v>
       </c>
       <c r="I182" s="1" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="J182" s="1" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="183" spans="1:10" ht="288" x14ac:dyDescent="0.2">
@@ -16218,16 +16215,16 @@
         <v>717</v>
       </c>
       <c r="F183" s="1" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G183" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H183" s="1" t="s">
         <v>1083</v>
       </c>
-      <c r="G183" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H183" s="1" t="s">
-        <v>1084</v>
-      </c>
       <c r="I183" s="1" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="J183" s="1" t="s">
         <v>925</v>
@@ -16244,22 +16241,22 @@
         <v>520</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>656</v>
       </c>
       <c r="F184" s="1" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G184" s="1" t="s">
         <v>1085</v>
       </c>
-      <c r="G184" s="1" t="s">
+      <c r="H184" s="1" t="s">
         <v>1086</v>
       </c>
-      <c r="H184" s="1" t="s">
+      <c r="I184" s="1" t="s">
         <v>1087</v>
-      </c>
-      <c r="I184" s="1" t="s">
-        <v>1088</v>
       </c>
       <c r="J184" s="1" t="s">
         <v>811</v>
@@ -16282,19 +16279,19 @@
         <v>656</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="G185" s="1" t="s">
         <v>759</v>
       </c>
       <c r="H185" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="I185" s="1" t="s">
         <v>1090</v>
       </c>
-      <c r="I185" s="1" t="s">
+      <c r="J185" s="1" t="s">
         <v>1091</v>
-      </c>
-      <c r="J185" s="1" t="s">
-        <v>1092</v>
       </c>
     </row>
     <row r="186" spans="1:10" ht="240" x14ac:dyDescent="0.2">
@@ -16308,13 +16305,13 @@
         <v>526</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E186" s="1" t="s">
         <v>656</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="G186" s="1" t="s">
         <v>656</v>
@@ -16355,10 +16352,10 @@
         <v>691</v>
       </c>
       <c r="I187" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="J187" s="1" t="s">
         <v>1094</v>
-      </c>
-      <c r="J187" s="1" t="s">
-        <v>1095</v>
       </c>
     </row>
     <row r="188" spans="1:10" ht="224" x14ac:dyDescent="0.2">
@@ -16378,7 +16375,7 @@
         <v>656</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="G188" s="1" t="s">
         <v>656</v>
@@ -16387,10 +16384,10 @@
         <v>688</v>
       </c>
       <c r="I188" s="1" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="J188" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="189" spans="1:10" ht="144" x14ac:dyDescent="0.2">
@@ -16413,10 +16410,10 @@
         <v>797</v>
       </c>
       <c r="G189" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="H189" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="I189" s="1" t="s">
         <v>752</v>
@@ -16474,13 +16471,13 @@
         <v>741</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="G191" s="1" t="s">
         <v>656</v>
       </c>
       <c r="H191" s="1" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="I191" s="1" t="s">
         <v>716</v>
@@ -16506,16 +16503,16 @@
         <v>656</v>
       </c>
       <c r="F192" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="G192" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H192" s="1" t="s">
         <v>1099</v>
       </c>
-      <c r="G192" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H192" s="1" t="s">
+      <c r="I192" s="1" t="s">
         <v>1100</v>
-      </c>
-      <c r="I192" s="1" t="s">
-        <v>1101</v>
       </c>
       <c r="J192" s="1" t="s">
         <v>761</v>
@@ -16544,7 +16541,7 @@
         <v>656</v>
       </c>
       <c r="H193" s="1" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I193" s="1" t="s">
         <v>925</v>
@@ -16570,13 +16567,13 @@
         <v>717</v>
       </c>
       <c r="F194" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G194" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="H194" s="1" t="s">
         <v>1102</v>
-      </c>
-      <c r="G194" s="1" t="s">
-        <v>1000</v>
-      </c>
-      <c r="H194" s="1" t="s">
-        <v>1103</v>
       </c>
       <c r="I194" s="1" t="s">
         <v>827</v>
@@ -16602,13 +16599,13 @@
         <v>656</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="G195" s="1" t="s">
         <v>656</v>
       </c>
       <c r="H195" s="1" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="I195" s="1" t="s">
         <v>665</v>
@@ -16628,7 +16625,7 @@
         <v>556</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E196" s="1" t="s">
         <v>656</v>
@@ -16643,7 +16640,7 @@
         <v>761</v>
       </c>
       <c r="I196" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="J196" s="1" t="s">
         <v>922</v>
@@ -16666,7 +16663,7 @@
         <v>656</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="G197" s="1" t="s">
         <v>755</v>
@@ -16698,16 +16695,16 @@
         <v>656</v>
       </c>
       <c r="F198" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="G198" s="1" t="s">
         <v>656</v>
       </c>
       <c r="H198" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="I198" s="1" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="J198" s="1" t="s">
         <v>877</v>
@@ -16730,7 +16727,7 @@
         <v>656</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="G199" s="1" t="s">
         <v>759</v>
@@ -16765,7 +16762,7 @@
         <v>729</v>
       </c>
       <c r="G200" s="1" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="H200" s="1" t="s">
         <v>720</v>
@@ -16774,7 +16771,7 @@
         <v>921</v>
       </c>
       <c r="J200" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="201" spans="1:10" ht="160" x14ac:dyDescent="0.2">
@@ -16794,16 +16791,16 @@
         <v>656</v>
       </c>
       <c r="F201" s="1" t="s">
+        <v>1107</v>
+      </c>
+      <c r="G201" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H201" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="I201" s="1" t="s">
         <v>1108</v>
-      </c>
-      <c r="G201" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H201" s="1" t="s">
-        <v>959</v>
-      </c>
-      <c r="I201" s="1" t="s">
-        <v>1109</v>
       </c>
       <c r="J201" s="1" t="s">
         <v>670</v>
@@ -16823,19 +16820,19 @@
         <v>655</v>
       </c>
       <c r="E202" s="1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="G202" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H202" s="1" t="s">
         <v>1110</v>
       </c>
-      <c r="F202" s="1" t="s">
-        <v>1041</v>
-      </c>
-      <c r="G202" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H202" s="1" t="s">
+      <c r="I202" s="1" t="s">
         <v>1111</v>
-      </c>
-      <c r="I202" s="1" t="s">
-        <v>1112</v>
       </c>
       <c r="J202" s="1" t="s">
         <v>688</v>
@@ -16858,19 +16855,19 @@
         <v>656</v>
       </c>
       <c r="F203" s="1" t="s">
+        <v>1112</v>
+      </c>
+      <c r="G203" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H203" s="1" t="s">
         <v>1113</v>
       </c>
-      <c r="G203" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H203" s="1" t="s">
+      <c r="I203" s="1" t="s">
         <v>1114</v>
       </c>
-      <c r="I203" s="1" t="s">
-        <v>1115</v>
-      </c>
       <c r="J203" s="1" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="204" spans="1:10" ht="288" x14ac:dyDescent="0.2">
@@ -16890,19 +16887,19 @@
         <v>656</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="G204" s="1" t="s">
         <v>656</v>
       </c>
       <c r="H204" s="1" t="s">
+        <v>1115</v>
+      </c>
+      <c r="I204" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="J204" s="1" t="s">
         <v>1116</v>
-      </c>
-      <c r="I204" s="1" t="s">
-        <v>1094</v>
-      </c>
-      <c r="J204" s="1" t="s">
-        <v>1117</v>
       </c>
     </row>
     <row r="205" spans="1:10" ht="335" x14ac:dyDescent="0.2">
@@ -16919,16 +16916,16 @@
         <v>655</v>
       </c>
       <c r="E205" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="F205" s="1" t="s">
         <v>1118</v>
       </c>
-      <c r="F205" s="1" t="s">
+      <c r="G205" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H205" s="1" t="s">
         <v>1119</v>
-      </c>
-      <c r="G205" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H205" s="1" t="s">
-        <v>1120</v>
       </c>
       <c r="I205" s="1" t="s">
         <v>901</v>
@@ -16954,19 +16951,19 @@
         <v>656</v>
       </c>
       <c r="F206" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="G206" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="H206" s="1" t="s">
         <v>756</v>
       </c>
       <c r="I206" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="J206" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="207" spans="1:10" ht="208" x14ac:dyDescent="0.2">
@@ -16986,7 +16983,7 @@
         <v>656</v>
       </c>
       <c r="F207" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="G207" s="1" t="s">
         <v>656</v>
@@ -16995,10 +16992,10 @@
         <v>709</v>
       </c>
       <c r="I207" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="J207" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="208" spans="1:10" ht="256" x14ac:dyDescent="0.2">
@@ -17018,13 +17015,13 @@
         <v>656</v>
       </c>
       <c r="F208" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="G208" s="1" t="s">
         <v>656</v>
       </c>
       <c r="H208" s="1" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I208" s="1" t="s">
         <v>955</v>
@@ -17050,10 +17047,10 @@
         <v>656</v>
       </c>
       <c r="F209" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="G209" s="1" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="H209" s="1" t="s">
         <v>656</v>
@@ -17082,7 +17079,7 @@
         <v>656</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="G210" s="1" t="s">
         <v>656</v>
@@ -17111,16 +17108,16 @@
         <v>655</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="G211" s="1" t="s">
         <v>656</v>
       </c>
       <c r="H211" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="I211" s="1" t="s">
         <v>904</v>
@@ -17152,7 +17149,7 @@
         <v>735</v>
       </c>
       <c r="H212" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="I212" s="1" t="s">
         <v>747</v>
@@ -17178,19 +17175,19 @@
         <v>656</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="G213" s="1" t="s">
         <v>677</v>
       </c>
       <c r="H213" s="1" t="s">
+        <v>1128</v>
+      </c>
+      <c r="I213" s="1" t="s">
         <v>1129</v>
       </c>
-      <c r="I213" s="1" t="s">
+      <c r="J213" s="1" t="s">
         <v>1130</v>
-      </c>
-      <c r="J213" s="1" t="s">
-        <v>1131</v>
       </c>
     </row>
     <row r="214" spans="1:10" ht="272" x14ac:dyDescent="0.2">
@@ -17210,19 +17207,19 @@
         <v>656</v>
       </c>
       <c r="F214" s="1" t="s">
+        <v>1131</v>
+      </c>
+      <c r="G214" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H214" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="I214" s="1" t="s">
         <v>1132</v>
       </c>
-      <c r="G214" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H214" s="1" t="s">
-        <v>965</v>
-      </c>
-      <c r="I214" s="1" t="s">
+      <c r="J214" s="1" t="s">
         <v>1133</v>
-      </c>
-      <c r="J214" s="1" t="s">
-        <v>1134</v>
       </c>
     </row>
     <row r="215" spans="1:10" ht="304" x14ac:dyDescent="0.2">
@@ -17254,7 +17251,7 @@
         <v>747</v>
       </c>
       <c r="J215" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="216" spans="1:10" ht="256" x14ac:dyDescent="0.2">
@@ -17274,19 +17271,19 @@
         <v>656</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="G216" s="1" t="s">
         <v>656</v>
       </c>
       <c r="H216" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="I216" s="1" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="J216" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="217" spans="1:10" ht="224" x14ac:dyDescent="0.2">
@@ -17306,7 +17303,7 @@
         <v>656</v>
       </c>
       <c r="F217" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="G217" s="1" t="s">
         <v>759</v>
@@ -17318,7 +17315,7 @@
         <v>929</v>
       </c>
       <c r="J217" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="218" spans="1:10" ht="272" x14ac:dyDescent="0.2">
@@ -17338,7 +17335,7 @@
         <v>656</v>
       </c>
       <c r="F218" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="G218" s="1" t="s">
         <v>755</v>
@@ -17370,13 +17367,13 @@
         <v>717</v>
       </c>
       <c r="F219" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="G219" s="1" t="s">
         <v>656</v>
       </c>
       <c r="H219" s="1" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I219" s="1" t="s">
         <v>733</v>
@@ -17405,13 +17402,13 @@
         <v>889</v>
       </c>
       <c r="G220" s="1" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H220" s="1" t="s">
         <v>1141</v>
       </c>
-      <c r="H220" s="1" t="s">
-        <v>1142</v>
-      </c>
       <c r="I220" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="J220" s="1" t="s">
         <v>771</v>
@@ -17434,19 +17431,19 @@
         <v>656</v>
       </c>
       <c r="F221" s="1" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G221" s="1" t="s">
         <v>1143</v>
       </c>
-      <c r="G221" s="1" t="s">
+      <c r="H221" s="1" t="s">
         <v>1144</v>
-      </c>
-      <c r="H221" s="1" t="s">
-        <v>1145</v>
       </c>
       <c r="I221" s="1" t="s">
         <v>747</v>
       </c>
       <c r="J221" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="222" spans="1:10" ht="240" x14ac:dyDescent="0.2">
@@ -17466,7 +17463,7 @@
         <v>656</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="G222" s="1" t="s">
         <v>677</v>
@@ -17475,7 +17472,7 @@
         <v>730</v>
       </c>
       <c r="I222" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="J222" s="1" t="s">
         <v>709</v>
@@ -17498,19 +17495,19 @@
         <v>656</v>
       </c>
       <c r="F223" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G223" s="1" t="s">
         <v>656</v>
       </c>
       <c r="H223" s="1" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I223" s="1" t="s">
         <v>688</v>
       </c>
       <c r="J223" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="224" spans="1:10" ht="256" x14ac:dyDescent="0.2">
@@ -17536,7 +17533,7 @@
         <v>656</v>
       </c>
       <c r="H224" s="1" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="I224" s="1" t="s">
         <v>939</v>
@@ -17562,13 +17559,13 @@
         <v>656</v>
       </c>
       <c r="F225" s="1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="G225" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="H225" s="1" t="s">
         <v>1150</v>
-      </c>
-      <c r="G225" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H225" s="1" t="s">
-        <v>1151</v>
       </c>
       <c r="I225" s="1" t="s">
         <v>863</v>

</xml_diff>